<commit_message>
Adds updated observations plots
</commit_message>
<xml_diff>
--- a/KF-ATTITUDE_RUNNING.xlsx
+++ b/KF-ATTITUDE_RUNNING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\KF-ATTITUDE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B9B7B0-D7D0-4C9C-A373-17AC10ECB3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF0E9E-57A6-4247-892A-F7FE9A6E212D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A53BC842-06E2-416D-B3BC-A55576E6EA79}"/>
   </bookViews>
@@ -1462,307 +1462,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1000.0277545245557</c:v>
+                  <c:v>999.99429493691491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>979.98696305694943</c:v>
+                  <c:v>980.00159951132457</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>960.40383290769796</c:v>
+                  <c:v>960.40614558592904</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>941.17669074285311</c:v>
+                  <c:v>941.18700843459624</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>922.36027612628686</c:v>
+                  <c:v>922.37600141655309</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>903.92350261007778</c:v>
+                  <c:v>903.92401846917005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>885.8293599771074</c:v>
+                  <c:v>885.83567637282476</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>868.1277468683079</c:v>
+                  <c:v>868.11012744809102</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>850.75995325543374</c:v>
+                  <c:v>850.77818573173465</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>833.7152681216628</c:v>
+                  <c:v>833.73110873752728</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>817.0683804504888</c:v>
+                  <c:v>817.04010610656815</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>800.73483260178921</c:v>
+                  <c:v>800.7352039632226</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>784.73267367475239</c:v>
+                  <c:v>784.69690387737126</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>769.02821184727065</c:v>
+                  <c:v>769.00884205896898</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>753.65945724087089</c:v>
+                  <c:v>753.62675446031096</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>738.56876403932631</c:v>
+                  <c:v>738.56726186376</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>723.80449284196038</c:v>
+                  <c:v>723.80347360387429</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>709.32083977128264</c:v>
+                  <c:v>709.33205720328624</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>695.12935228276626</c:v>
+                  <c:v>695.12115713393564</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>681.22918093055569</c:v>
+                  <c:v>681.22713487978695</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>667.60337902536105</c:v>
+                  <c:v>667.58609972483566</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>654.25620055721834</c:v>
+                  <c:v>654.25718237706508</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>641.16146071678713</c:v>
+                  <c:v>641.1637557699604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>628.35331858720849</c:v>
+                  <c:v>628.34705587576457</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>615.78113456076801</c:v>
+                  <c:v>615.78305131594323</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>603.44983210320788</c:v>
+                  <c:v>603.46056809394929</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>591.38839462802673</c:v>
+                  <c:v>591.38757620180093</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>579.57564708117752</c:v>
+                  <c:v>579.57184547796385</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>567.97785124513825</c:v>
+                  <c:v>567.97692332281861</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>556.61670598550438</c:v>
+                  <c:v>556.62136163230343</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>545.47390146621308</c:v>
+                  <c:v>545.48579064923013</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>534.57098440829441</c:v>
+                  <c:v>534.58257171049229</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>523.87944407866485</c:v>
+                  <c:v>523.87645790302963</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>513.40665870443809</c:v>
+                  <c:v>513.41028933529867</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>503.13678648242302</c:v>
+                  <c:v>503.14009940682854</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>493.07311093411488</c:v>
+                  <c:v>493.07903085181289</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>483.21201143745446</c:v>
+                  <c:v>483.21360791187419</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>473.54909169003116</c:v>
+                  <c:v>473.54744338841692</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>464.07886953656379</c:v>
+                  <c:v>464.08469781016635</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>454.80526695933906</c:v>
+                  <c:v>454.80147926252567</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>445.69954924182241</c:v>
+                  <c:v>445.69907200671878</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>436.79457339888774</c:v>
+                  <c:v>436.78698134042247</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>428.04868908641265</c:v>
+                  <c:v>428.05020520666045</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>419.48888456030801</c:v>
+                  <c:v>419.49446984529942</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>411.09722507557626</c:v>
+                  <c:v>411.09413984061223</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>402.87910045302203</c:v>
+                  <c:v>402.8827253775703</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>394.82068830724853</c:v>
+                  <c:v>394.81669587664481</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>386.9268431220089</c:v>
+                  <c:v>386.92453605361561</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>379.18096107050184</c:v>
+                  <c:v>379.18202995825294</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>371.60102035950865</c:v>
+                  <c:v>371.60059580453873</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>364.17141276965492</c:v>
+                  <c:v>364.168831259294</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>356.88941860765397</c:v>
+                  <c:v>356.88889087844228</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>349.74424920509023</c:v>
+                  <c:v>349.74814464684732</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>342.75552448228706</c:v>
+                  <c:v>342.75157247733972</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>335.900022741481</c:v>
+                  <c:v>335.89674471868102</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>329.18336333305376</c:v>
+                  <c:v>329.18133224202688</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>322.59660376411898</c:v>
+                  <c:v>322.59422640075508</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>316.14481374199249</c:v>
+                  <c:v>316.14460192027565</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>309.82118431443712</c:v>
+                  <c:v>309.82383126522012</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>303.62787367370089</c:v>
+                  <c:v>303.62735633722258</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>297.55122965141118</c:v>
+                  <c:v>297.55168351185876</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>291.60073704200255</c:v>
+                  <c:v>291.60265975360153</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>285.76875479175101</c:v>
+                  <c:v>285.76946089988621</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>280.05378502331212</c:v>
+                  <c:v>280.05377099553846</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>274.45462150684654</c:v>
+                  <c:v>274.45266931039339</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>268.96651864089324</c:v>
+                  <c:v>268.9639466305357</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>263.58387003997547</c:v>
+                  <c:v>263.58410171103992</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>258.31312832069187</c:v>
+                  <c:v>258.31423719521837</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>253.14759430719084</c:v>
+                  <c:v>253.1503785702958</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>248.08096573753073</c:v>
+                  <c:v>248.08438881567633</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>243.12200812626361</c:v>
+                  <c:v>243.12260225276569</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>238.26000493870006</c:v>
+                  <c:v>238.26071579220385</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>233.49482898438669</c:v>
+                  <c:v>233.49461499949115</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>228.82444112151222</c:v>
+                  <c:v>228.82306786383944</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>224.24789173435261</c:v>
+                  <c:v>224.24787976332044</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>219.76364503610719</c:v>
+                  <c:v>219.76439961263969</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>215.3686725459109</c:v>
+                  <c:v>215.36828263034454</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>211.06139705357035</c:v>
+                  <c:v>211.06160834482216</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>206.83916254293916</c:v>
+                  <c:v>206.83990495343733</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>202.70480988045804</c:v>
+                  <c:v>202.70191004115776</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>198.64759479152008</c:v>
+                  <c:v>198.64818697655269</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>194.67593059041283</c:v>
+                  <c:v>194.67708606261135</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>190.78310626250317</c:v>
+                  <c:v>190.7803277505673</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>186.96521294438622</c:v>
+                  <c:v>186.96769345681201</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>183.2268892292025</c:v>
+                  <c:v>183.22757414943607</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>179.56223581289302</c:v>
+                  <c:v>179.56256399336266</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>175.97207777662499</c:v>
+                  <c:v>175.97155624181545</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>172.4522276201192</c:v>
+                  <c:v>172.4510056319094</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>169.00315370736158</c:v>
+                  <c:v>169.00285700064046</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>165.62353059275085</c:v>
+                  <c:v>165.62230841384945</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>162.31132610577157</c:v>
+                  <c:v>162.31118187184373</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>159.0637101379852</c:v>
+                  <c:v>159.06308067035528</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>155.88281874818503</c:v>
+                  <c:v>155.88324301820285</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>152.76542197219106</c:v>
+                  <c:v>152.7651886495162</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>149.70943208697656</c:v>
+                  <c:v>149.70969116985091</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>146.71583766014101</c:v>
+                  <c:v>146.71555054542526</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>143.78134062843822</c:v>
+                  <c:v>143.78206484364264</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>140.90496676395557</c:v>
+                  <c:v>140.90591271037292</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>138.08750101252139</c:v>
+                  <c:v>138.08793377653473</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>135.32530075047043</c:v>
+                  <c:v>135.32612530940864</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>132.61948668724938</c:v>
+                  <c:v>132.61942558987562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2132,307 +2132,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1069.4140659136519</c:v>
+                  <c:v>985.73163722427773</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>946.05073062625274</c:v>
+                  <c:v>984.16525872782631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>970.79260136323273</c:v>
+                  <c:v>977.06323056443966</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>897.97132634173249</c:v>
+                  <c:v>927.09994985730009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>899.19320872950334</c:v>
+                  <c:v>945.41830680877956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>912.20247743029563</c:v>
+                  <c:v>913.78136882689193</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>844.34659779480808</c:v>
+                  <c:v>864.47608579593691</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>875.47082806566982</c:v>
+                  <c:v>817.00562482884607</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>840.15848870147283</c:v>
+                  <c:v>903.15176165584819</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>716.85310098497973</c:v>
+                  <c:v>773.83848106058247</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>800.4926457186707</c:v>
+                  <c:v>694.58507874762893</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>814.31098328529367</c:v>
+                  <c:v>815.75933657897701</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>849.4876642407603</c:v>
+                  <c:v>704.23047675419423</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>793.64197626099269</c:v>
+                  <c:v>711.74089438394185</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>830.75673134686269</c:v>
+                  <c:v>686.77969628304481</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>737.01690422719923</c:v>
+                  <c:v>730.13080650564416</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>756.1220506302252</c:v>
+                  <c:v>751.25716955155644</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>704.71767658962233</c:v>
+                  <c:v>760.46631643102603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>664.1979996481906</c:v>
+                  <c:v>621.79055894798046</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>662.67998141611156</c:v>
+                  <c:v>651.65580513532882</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>641.8420733787276</c:v>
+                  <c:v>544.9026218510952</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>656.52367293318036</c:v>
+                  <c:v>662.25890492601548</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>584.99897034516152</c:v>
+                  <c:v>598.9580517428567</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>666.57599217531572</c:v>
+                  <c:v>626.91427524147844</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>621.04275355969378</c:v>
+                  <c:v>633.68199139686772</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>501.17830523481865</c:v>
+                  <c:v>574.89088495729641</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>541.06256000082647</c:v>
+                  <c:v>535.21163725946201</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>640.01504392454069</c:v>
+                  <c:v>611.71695838749019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>580.9607324336572</c:v>
+                  <c:v>573.76876970290459</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>557.04884467698184</c:v>
+                  <c:v>594.62059796392191</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>457.94402252187012</c:v>
+                  <c:v>557.84716902328785</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>502.65208104737826</c:v>
+                  <c:v>604.03278203535581</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>490.21021026409778</c:v>
+                  <c:v>463.00612127302514</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>524.60964272737738</c:v>
+                  <c:v>559.04835427331307</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>497.39412784152142</c:v>
+                  <c:v>530.11481094451142</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>477.54921395796953</c:v>
+                  <c:v>538.42892911840727</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>471.25491803241056</c:v>
+                  <c:v>488.34975972646356</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>476.06915760682887</c:v>
+                  <c:v>457.69167393355718</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>475.46875207215737</c:v>
+                  <c:v>543.12931376765732</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>562.8164109201241</c:v>
+                  <c:v>517.03204082789512</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>434.94301669787649</c:v>
+                  <c:v>428.93652554092296</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>543.95237278697903</c:v>
+                  <c:v>444.45892365500316</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>401.04851938459512</c:v>
+                  <c:v>421.7363583499835</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>408.54911892330153</c:v>
+                  <c:v>487.9039562145141</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>372.09752656084822</c:v>
+                  <c:v>326.45570696660252</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>421.91944345157697</c:v>
+                  <c:v>477.75622313648375</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>400.93615806504363</c:v>
+                  <c:v>336.90291472625688</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>436.05969575204949</c:v>
+                  <c:v>397.53179295702768</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>301.60216794463219</c:v>
+                  <c:v>320.18850545311403</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>359.03628023175776</c:v>
+                  <c:v>351.34953463701049</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>396.83406433924364</c:v>
+                  <c:v>348.16764996682815</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>418.36731473392291</c:v>
+                  <c:v>408.00841694084153</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>261.62685990197912</c:v>
+                  <c:v>341.24391346657166</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>383.93149810226475</c:v>
+                  <c:v>299.8280362059898</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>369.24711336787686</c:v>
+                  <c:v>296.61053072919367</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>394.15066334134872</c:v>
+                  <c:v>347.28876326851611</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>314.60470833591404</c:v>
+                  <c:v>257.49194479035998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>311.54300705925004</c:v>
+                  <c:v>306.24447915543891</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>286.03090230649184</c:v>
+                  <c:v>354.97193257746295</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>363.77269867279796</c:v>
+                  <c:v>349.74287561438211</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>243.53364795753242</c:v>
+                  <c:v>256.34953417444706</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>252.1214862698701</c:v>
+                  <c:v>308.65261953134859</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>246.4784410847372</c:v>
+                  <c:v>268.09527193543693</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>252.88156619636953</c:v>
+                  <c:v>252.43441247968198</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>310.19253379845071</c:v>
+                  <c:v>245.39791718902953</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>339.63125863552636</c:v>
+                  <c:v>250.74483170703402</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>216.2907675906464</c:v>
+                  <c:v>224.62723162125354</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>245.11179331289037</c:v>
+                  <c:v>286.65881187389135</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>268.09885596521781</c:v>
+                  <c:v>376.72018674516892</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>113.98990539285595</c:v>
+                  <c:v>253.03928910866867</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>218.87124349588515</c:v>
+                  <c:v>244.00044015569645</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>232.75825873226557</c:v>
+                  <c:v>264.06423345282059</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>228.98794243493762</c:v>
+                  <c:v>219.17548696279601</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>200.76898825744186</c:v>
+                  <c:v>135.2006635075289</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>192.60894910462102</c:v>
+                  <c:v>192.0138063652694</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>224.29034650028439</c:v>
+                  <c:v>263.35107501942292</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>236.17942585802246</c:v>
+                  <c:v>215.16318028052217</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>237.79437967642488</c:v>
+                  <c:v>249.65243867126176</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>175.29893882706904</c:v>
+                  <c:v>218.68235401615215</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>318.40840772022221</c:v>
+                  <c:v>141.96675450150101</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>119.1210439311043</c:v>
+                  <c:v>156.63839605586628</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>198.46959763746335</c:v>
+                  <c:v>274.69185923681141</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>242.34127050600839</c:v>
+                  <c:v>51.495655933046805</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>80.006572438209929</c:v>
+                  <c:v>257.40874052062446</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>147.10279969507633</c:v>
+                  <c:v>198.10690344550534</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>133.73522111379049</c:v>
+                  <c:v>159.18156981791788</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>216.94154104900849</c:v>
+                  <c:v>174.83557176385818</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>179.909740641865</c:v>
+                  <c:v>77.18500786965501</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>174.04298591407817</c:v>
+                  <c:v>148.07232315640726</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>210.86316026523892</c:v>
+                  <c:v>99.475243194867275</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>233.72831119214987</c:v>
+                  <c:v>220.04099212903719</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>94.649165445573999</c:v>
+                  <c:v>32.45179422653473</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>129.53849772830455</c:v>
+                  <c:v>173.18893963559157</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>153.69294342613375</c:v>
+                  <c:v>128.69807064694817</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>74.646171955091972</c:v>
+                  <c:v>103.54500983622921</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>139.1333979142895</c:v>
+                  <c:v>105.78731553062633</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>114.24310718537326</c:v>
+                  <c:v>201.82305968251325</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>16.698035630948922</c:v>
+                  <c:v>135.80888185352947</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>94.413641558896984</c:v>
+                  <c:v>151.15289603363891</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>29.295853024814804</c:v>
+                  <c:v>141.860472266101</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>122.78213825226823</c:v>
+                  <c:v>114.09752529818294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3072,307 +3072,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1069.4140659136519</c:v>
+                  <c:v>985.73163722427773</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>946.05073062625274</c:v>
+                  <c:v>984.16525872782631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>970.79260136323273</c:v>
+                  <c:v>977.06323056443966</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>897.97132634173249</c:v>
+                  <c:v>927.09994985730009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>899.19320872950334</c:v>
+                  <c:v>945.41830680877956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>912.20247743029563</c:v>
+                  <c:v>913.78136882689193</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>844.34659779480808</c:v>
+                  <c:v>864.47608579593691</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>875.47082806566982</c:v>
+                  <c:v>817.00562482884607</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>840.15848870147283</c:v>
+                  <c:v>903.15176165584819</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>716.85310098497973</c:v>
+                  <c:v>773.83848106058247</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>800.4926457186707</c:v>
+                  <c:v>694.58507874762893</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>814.31098328529367</c:v>
+                  <c:v>815.75933657897701</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>849.4876642407603</c:v>
+                  <c:v>704.23047675419423</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>793.64197626099269</c:v>
+                  <c:v>711.74089438394185</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>830.75673134686269</c:v>
+                  <c:v>686.77969628304481</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>737.01690422719923</c:v>
+                  <c:v>730.13080650564416</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>756.1220506302252</c:v>
+                  <c:v>751.25716955155644</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>704.71767658962233</c:v>
+                  <c:v>760.46631643102603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>664.1979996481906</c:v>
+                  <c:v>621.79055894798046</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>662.67998141611156</c:v>
+                  <c:v>651.65580513532882</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>641.8420733787276</c:v>
+                  <c:v>544.9026218510952</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>656.52367293318036</c:v>
+                  <c:v>662.25890492601548</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>584.99897034516152</c:v>
+                  <c:v>598.9580517428567</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>666.57599217531572</c:v>
+                  <c:v>626.91427524147844</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>621.04275355969378</c:v>
+                  <c:v>633.68199139686772</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>501.17830523481865</c:v>
+                  <c:v>574.89088495729641</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>541.06256000082647</c:v>
+                  <c:v>535.21163725946201</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>640.01504392454069</c:v>
+                  <c:v>611.71695838749019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>580.9607324336572</c:v>
+                  <c:v>573.76876970290459</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>557.04884467698184</c:v>
+                  <c:v>594.62059796392191</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>457.94402252187012</c:v>
+                  <c:v>557.84716902328785</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>502.65208104737826</c:v>
+                  <c:v>604.03278203535581</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>490.21021026409778</c:v>
+                  <c:v>463.00612127302514</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>524.60964272737738</c:v>
+                  <c:v>559.04835427331307</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>497.39412784152142</c:v>
+                  <c:v>530.11481094451142</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>477.54921395796953</c:v>
+                  <c:v>538.42892911840727</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>471.25491803241056</c:v>
+                  <c:v>488.34975972646356</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>476.06915760682887</c:v>
+                  <c:v>457.69167393355718</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>475.46875207215737</c:v>
+                  <c:v>543.12931376765732</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>562.8164109201241</c:v>
+                  <c:v>517.03204082789512</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>434.94301669787649</c:v>
+                  <c:v>428.93652554092296</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>543.95237278697903</c:v>
+                  <c:v>444.45892365500316</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>401.04851938459512</c:v>
+                  <c:v>421.7363583499835</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>408.54911892330153</c:v>
+                  <c:v>487.9039562145141</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>372.09752656084822</c:v>
+                  <c:v>326.45570696660252</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>421.91944345157697</c:v>
+                  <c:v>477.75622313648375</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>400.93615806504363</c:v>
+                  <c:v>336.90291472625688</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>436.05969575204949</c:v>
+                  <c:v>397.53179295702768</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>301.60216794463219</c:v>
+                  <c:v>320.18850545311403</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>359.03628023175776</c:v>
+                  <c:v>351.34953463701049</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>396.83406433924364</c:v>
+                  <c:v>348.16764996682815</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>418.36731473392291</c:v>
+                  <c:v>408.00841694084153</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>261.62685990197912</c:v>
+                  <c:v>341.24391346657166</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>383.93149810226475</c:v>
+                  <c:v>299.8280362059898</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>369.24711336787686</c:v>
+                  <c:v>296.61053072919367</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>394.15066334134872</c:v>
+                  <c:v>347.28876326851611</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>314.60470833591404</c:v>
+                  <c:v>257.49194479035998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>311.54300705925004</c:v>
+                  <c:v>306.24447915543891</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>286.03090230649184</c:v>
+                  <c:v>354.97193257746295</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>363.77269867279796</c:v>
+                  <c:v>349.74287561438211</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>243.53364795753242</c:v>
+                  <c:v>256.34953417444706</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>252.1214862698701</c:v>
+                  <c:v>308.65261953134859</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>246.4784410847372</c:v>
+                  <c:v>268.09527193543693</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>252.88156619636953</c:v>
+                  <c:v>252.43441247968198</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>310.19253379845071</c:v>
+                  <c:v>245.39791718902953</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>339.63125863552636</c:v>
+                  <c:v>250.74483170703402</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>216.2907675906464</c:v>
+                  <c:v>224.62723162125354</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>245.11179331289037</c:v>
+                  <c:v>286.65881187389135</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>268.09885596521781</c:v>
+                  <c:v>376.72018674516892</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>113.98990539285595</c:v>
+                  <c:v>253.03928910866867</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>218.87124349588515</c:v>
+                  <c:v>244.00044015569645</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>232.75825873226557</c:v>
+                  <c:v>264.06423345282059</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>228.98794243493762</c:v>
+                  <c:v>219.17548696279601</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>200.76898825744186</c:v>
+                  <c:v>135.2006635075289</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>192.60894910462102</c:v>
+                  <c:v>192.0138063652694</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>224.29034650028439</c:v>
+                  <c:v>263.35107501942292</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>236.17942585802246</c:v>
+                  <c:v>215.16318028052217</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>237.79437967642488</c:v>
+                  <c:v>249.65243867126176</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>175.29893882706904</c:v>
+                  <c:v>218.68235401615215</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>318.40840772022221</c:v>
+                  <c:v>141.96675450150101</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>119.1210439311043</c:v>
+                  <c:v>156.63839605586628</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>198.46959763746335</c:v>
+                  <c:v>274.69185923681141</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>242.34127050600839</c:v>
+                  <c:v>51.495655933046805</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>80.006572438209929</c:v>
+                  <c:v>257.40874052062446</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>147.10279969507633</c:v>
+                  <c:v>198.10690344550534</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>133.73522111379049</c:v>
+                  <c:v>159.18156981791788</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>216.94154104900849</c:v>
+                  <c:v>174.83557176385818</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>179.909740641865</c:v>
+                  <c:v>77.18500786965501</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>174.04298591407817</c:v>
+                  <c:v>148.07232315640726</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>210.86316026523892</c:v>
+                  <c:v>99.475243194867275</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>233.72831119214987</c:v>
+                  <c:v>220.04099212903719</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>94.649165445573999</c:v>
+                  <c:v>32.45179422653473</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>129.53849772830455</c:v>
+                  <c:v>173.18893963559157</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>153.69294342613375</c:v>
+                  <c:v>128.69807064694817</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>74.646171955091972</c:v>
+                  <c:v>103.54500983622921</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>139.1333979142895</c:v>
+                  <c:v>105.78731553062633</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>114.24310718537326</c:v>
+                  <c:v>201.82305968251325</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>16.698035630948922</c:v>
+                  <c:v>135.80888185352947</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>94.413641558896984</c:v>
+                  <c:v>151.15289603363891</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>29.295853024814804</c:v>
+                  <c:v>141.860472266101</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>122.78213825226823</c:v>
+                  <c:v>114.09752529818294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5307,11 +5307,11 @@
       </c>
       <c r="E13">
         <f ca="1">IF($K$3=0,$K$2,NORMINV(RAND(),$K$2,$K$3))</f>
-        <v>89.414065913651825</v>
+        <v>5.7316372242777236</v>
       </c>
       <c r="F13">
         <f ca="1">D13+E13</f>
-        <v>1069.4140659136519</v>
+        <v>985.73163722427773</v>
       </c>
       <c r="G13" s="18">
         <f>E2</f>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="J13" s="9">
         <f ca="1">G13+I13*(F13-G13)</f>
-        <v>1000.0277545245557</v>
+        <v>999.99429493691491</v>
       </c>
       <c r="K13" s="19">
         <f>(1-I13)*H13</f>
@@ -5347,11 +5347,11 @@
       </c>
       <c r="E14">
         <f t="shared" ref="E14:E77" ca="1" si="2">IF($K$3=0,$K$2,NORMINV(RAND(),$K$2,$K$3))</f>
-        <v>-14.349269373747267</v>
+        <v>23.765258727826318</v>
       </c>
       <c r="F14">
         <f t="shared" ref="F14:F77" ca="1" si="3">D14+E14</f>
-        <v>946.05073062625274</v>
+        <v>984.16525872782631</v>
       </c>
       <c r="G14" s="18">
         <f>$B$2*G13</f>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="J14" s="9">
         <f t="shared" ref="J14:J77" ca="1" si="4">G14+I14*(F14-G14)</f>
-        <v>979.98696305694943</v>
+        <v>980.00159951132457</v>
       </c>
       <c r="K14" s="19">
         <f t="shared" ref="K14:K77" si="5">(1-I14)*H14</f>
@@ -5388,11 +5388,11 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
-        <v>29.600601363232776</v>
+        <v>35.871230564439621</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="3"/>
-        <v>970.79260136323273</v>
+        <v>977.06323056443966</v>
       </c>
       <c r="G15" s="18">
         <f t="shared" ref="G15:G78" si="6">$B$2*G14</f>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="J15" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>960.40383290769796</v>
+        <v>960.40614558592904</v>
       </c>
       <c r="K15" s="19">
         <f t="shared" si="5"/>
@@ -5429,11 +5429,11 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>-24.396833658267518</v>
+        <v>4.7317898573001003</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="3"/>
-        <v>897.97132634173249</v>
+        <v>927.09994985730009</v>
       </c>
       <c r="G16" s="18">
         <f t="shared" si="6"/>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="J16" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>941.17669074285311</v>
+        <v>941.18700843459624</v>
       </c>
       <c r="K16" s="19">
         <f t="shared" si="5"/>
@@ -5470,11 +5470,11 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>-4.7275880704966449</v>
+        <v>41.497510008779656</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="3"/>
-        <v>899.19320872950334</v>
+        <v>945.41830680877956</v>
       </c>
       <c r="G17" s="18">
         <f t="shared" si="6"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="J17" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>922.36027612628686</v>
+        <v>922.37600141655309</v>
       </c>
       <c r="K17" s="19">
         <f t="shared" si="5"/>
@@ -5511,11 +5511,11 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
-        <v>26.360096566295756</v>
+        <v>27.938987962892032</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="3"/>
-        <v>912.20247743029563</v>
+        <v>913.78136882689193</v>
       </c>
       <c r="G18" s="18">
         <f t="shared" si="6"/>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="J18" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>903.92350261007778</v>
+        <v>903.92401846917005</v>
       </c>
       <c r="K18" s="19">
         <f t="shared" si="5"/>
@@ -5552,11 +5552,11 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
-        <v>-23.77893545191186</v>
+        <v>-3.6494474507829548</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="3"/>
-        <v>844.34659779480808</v>
+        <v>864.47608579593691</v>
       </c>
       <c r="G19" s="18">
         <f t="shared" si="6"/>
@@ -5572,7 +5572,7 @@
       </c>
       <c r="J19" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>885.8293599771074</v>
+        <v>885.83567637282476</v>
       </c>
       <c r="K19" s="19">
         <f t="shared" si="5"/>
@@ -5593,11 +5593,11 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
-        <v>24.707805483884439</v>
+        <v>-33.757397752939333</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="3"/>
-        <v>875.47082806566982</v>
+        <v>817.00562482884607</v>
       </c>
       <c r="G20" s="18">
         <f t="shared" si="6"/>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="J20" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>868.1277468683079</v>
+        <v>868.11012744809102</v>
       </c>
       <c r="K20" s="19">
         <f t="shared" si="5"/>
@@ -5634,11 +5634,11 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>6.4107265713231572</v>
+        <v>69.403999525698552</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="3"/>
-        <v>840.15848870147283</v>
+        <v>903.15176165584819</v>
       </c>
       <c r="G21" s="18">
         <f t="shared" si="6"/>
@@ -5654,7 +5654,7 @@
       </c>
       <c r="J21" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>850.75995325543374</v>
+        <v>850.77818573173465</v>
       </c>
       <c r="K21" s="19">
         <f t="shared" si="5"/>
@@ -5675,11 +5675,11 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
-        <v>-100.21970590256699</v>
+        <v>-43.234325826964223</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="3"/>
-        <v>716.85310098497973</v>
+        <v>773.83848106058247</v>
       </c>
       <c r="G22" s="18">
         <f t="shared" si="6"/>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="J22" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>833.7152681216628</v>
+        <v>833.73110873752728</v>
       </c>
       <c r="K22" s="19">
         <f t="shared" si="5"/>
@@ -5716,11 +5716,11 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.23870503112509528</v>
+        <v>-106.14627200216682</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="3"/>
-        <v>800.4926457186707</v>
+        <v>694.58507874762893</v>
       </c>
       <c r="G23" s="18">
         <f t="shared" si="6"/>
@@ -5736,7 +5736,7 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>817.0683804504888</v>
+        <v>817.04010610656815</v>
       </c>
       <c r="K23" s="19">
         <f t="shared" si="5"/>
@@ -5757,11 +5757,11 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
-        <v>29.594259550493764</v>
+        <v>31.042612844177192</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="3"/>
-        <v>814.31098328529367</v>
+        <v>815.75933657897701</v>
       </c>
       <c r="G24" s="18">
         <f t="shared" si="6"/>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="J24" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>800.73483260178921</v>
+        <v>800.7352039632226</v>
       </c>
       <c r="K24" s="19">
         <f t="shared" si="5"/>
@@ -5798,11 +5798,11 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>80.465274980656488</v>
+        <v>-64.791912505909679</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="3"/>
-        <v>849.4876642407603</v>
+        <v>704.23047675419423</v>
       </c>
       <c r="G25" s="18">
         <f t="shared" si="6"/>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="J25" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>784.73267367475239</v>
+        <v>784.69690387737126</v>
       </c>
       <c r="K25" s="19">
         <f t="shared" si="5"/>
@@ -5839,11 +5839,11 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>40.000034786090993</v>
+        <v>-41.901047090959871</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="3"/>
-        <v>793.64197626099269</v>
+        <v>711.74089438394185</v>
       </c>
       <c r="G26" s="18">
         <f t="shared" si="6"/>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="J26" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>769.02821184727065</v>
+        <v>769.00884205896898</v>
       </c>
       <c r="K26" s="19">
         <f t="shared" si="5"/>
@@ -5880,11 +5880,11 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
-        <v>92.187628701459033</v>
+        <v>-51.789406362358761</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="3"/>
-        <v>830.75673134686269</v>
+        <v>686.77969628304481</v>
       </c>
       <c r="G27" s="18">
         <f t="shared" si="6"/>
@@ -5900,7 +5900,7 @@
       </c>
       <c r="J27" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>753.65945724087089</v>
+        <v>753.62675446031096</v>
       </c>
       <c r="K27" s="19">
         <f t="shared" si="5"/>
@@ -5921,11 +5921,11 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="2"/>
-        <v>13.21918363470369</v>
+        <v>6.3330859131485377</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="3"/>
-        <v>737.01690422719923</v>
+        <v>730.13080650564416</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="6"/>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="J28" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>738.56876403932631</v>
+        <v>738.56726186376</v>
       </c>
       <c r="K28" s="19">
         <f t="shared" si="5"/>
@@ -5962,11 +5962,11 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
-        <v>46.800284449579578</v>
+        <v>41.935403370910819</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="3"/>
-        <v>756.1220506302252</v>
+        <v>751.25716955155644</v>
       </c>
       <c r="G29" s="18">
         <f t="shared" si="6"/>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="J29" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>723.80449284196038</v>
+        <v>723.80347360387429</v>
       </c>
       <c r="K29" s="19">
         <f t="shared" si="5"/>
@@ -6003,11 +6003,11 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>9.5823457325895838</v>
+        <v>65.330985573993274</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="3"/>
-        <v>704.71767658962233</v>
+        <v>760.46631643102603</v>
       </c>
       <c r="G30" s="18">
         <f t="shared" si="6"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="J30" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>709.32083977128264</v>
+        <v>709.33205720328624</v>
       </c>
       <c r="K30" s="19">
         <f t="shared" si="5"/>
@@ -6044,11 +6044,11 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>-17.034624591701416</v>
+        <v>-59.442065291911582</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="3"/>
-        <v>664.1979996481906</v>
+        <v>621.79055894798046</v>
       </c>
       <c r="G31" s="18">
         <f t="shared" si="6"/>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="J31" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>695.12935228276626</v>
+        <v>695.12115713393564</v>
       </c>
       <c r="K31" s="19">
         <f t="shared" si="5"/>
@@ -6085,11 +6085,11 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>-4.9279903389826751</v>
+        <v>-15.952166619765421</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="3"/>
-        <v>662.67998141611156</v>
+        <v>651.65580513532882</v>
       </c>
       <c r="G32" s="18">
         <f t="shared" si="6"/>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="J32" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>681.22918093055569</v>
+        <v>681.22713487978695</v>
       </c>
       <c r="K32" s="19">
         <f t="shared" si="5"/>
@@ -6126,11 +6126,11 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="2"/>
-        <v>-12.41373894126469</v>
+        <v>-109.35319046889708</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="3"/>
-        <v>641.8420733787276</v>
+        <v>544.9026218510952</v>
       </c>
       <c r="G33" s="18">
         <f t="shared" si="6"/>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="J33" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>667.60337902536105</v>
+        <v>667.58609972483566</v>
       </c>
       <c r="K33" s="19">
         <f t="shared" si="5"/>
@@ -6167,11 +6167,11 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="2"/>
-        <v>15.352976859587889</v>
+        <v>21.088208852423005</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="3"/>
-        <v>656.52367293318036</v>
+        <v>662.25890492601548</v>
       </c>
       <c r="G34" s="18">
         <f t="shared" si="6"/>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="J34" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>654.25620055721834</v>
+        <v>654.25718237706508</v>
       </c>
       <c r="K34" s="19">
         <f t="shared" si="5"/>
@@ -6208,11 +6208,11 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="2"/>
-        <v>-43.348311806959053</v>
+        <v>-29.389230409263838</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="3"/>
-        <v>584.99897034516152</v>
+        <v>598.9580517428567</v>
       </c>
       <c r="G35" s="18">
         <f t="shared" si="6"/>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="J35" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>641.16146071678713</v>
+        <v>641.1637557699604</v>
       </c>
       <c r="K35" s="19">
         <f t="shared" si="5"/>
@@ -6249,11 +6249,11 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="2"/>
-        <v>50.795655666237607</v>
+        <v>11.133938732400335</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="3"/>
-        <v>666.57599217531572</v>
+        <v>626.91427524147844</v>
       </c>
       <c r="G36" s="18">
         <f t="shared" si="6"/>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="J36" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>628.35331858720849</v>
+        <v>628.34705587576457</v>
       </c>
       <c r="K36" s="19">
         <f t="shared" si="5"/>
@@ -6290,11 +6290,11 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="2"/>
-        <v>17.578023780797256</v>
+        <v>30.217261617971182</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="3"/>
-        <v>621.04275355969378</v>
+        <v>633.68199139686772</v>
       </c>
       <c r="G37" s="18">
         <f t="shared" si="6"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="J37" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>615.78113456076801</v>
+        <v>615.78305131594323</v>
       </c>
       <c r="K37" s="19">
         <f t="shared" si="5"/>
@@ -6331,11 +6331,11 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="2"/>
-        <v>-90.217129948499903</v>
+        <v>-16.50455022602214</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="3"/>
-        <v>501.17830523481865</v>
+        <v>574.89088495729641</v>
       </c>
       <c r="G38" s="18">
         <f t="shared" si="6"/>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="J38" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>603.44983210320788</v>
+        <v>603.46056809394929</v>
       </c>
       <c r="K38" s="19">
         <f t="shared" si="5"/>
@@ -6372,11 +6372,11 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="2"/>
-        <v>-38.504966478825715</v>
+        <v>-44.355889220190178</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="3"/>
-        <v>541.06256000082647</v>
+        <v>535.21163725946201</v>
       </c>
       <c r="G39" s="18">
         <f t="shared" si="6"/>
@@ -6392,7 +6392,7 @@
       </c>
       <c r="J39" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>591.38839462802673</v>
+        <v>591.38757620180093</v>
       </c>
       <c r="K39" s="19">
         <f t="shared" si="5"/>
@@ -6413,11 +6413,11 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="2"/>
-        <v>72.038867974481533</v>
+        <v>43.740782437431037</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="3"/>
-        <v>640.01504392454069</v>
+        <v>611.71695838749019</v>
       </c>
       <c r="G40" s="18">
         <f t="shared" si="6"/>
@@ -6433,7 +6433,7 @@
       </c>
       <c r="J40" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>579.57564708117752</v>
+        <v>579.57184547796385</v>
       </c>
       <c r="K40" s="19">
         <f t="shared" si="5"/>
@@ -6454,11 +6454,11 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="2"/>
-        <v>24.34408000259916</v>
+        <v>17.152117271846546</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="3"/>
-        <v>580.9607324336572</v>
+        <v>573.76876970290459</v>
       </c>
       <c r="G41" s="18">
         <f t="shared" si="6"/>
@@ -6474,7 +6474,7 @@
       </c>
       <c r="J41" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>567.97785124513825</v>
+        <v>567.97692332281861</v>
       </c>
       <c r="K41" s="19">
         <f t="shared" si="5"/>
@@ -6495,11 +6495,11 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="2"/>
-        <v>11.564525294545016</v>
+        <v>49.136278581484987</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="3"/>
-        <v>557.04884467698184</v>
+        <v>594.62059796392191</v>
       </c>
       <c r="G42" s="18">
         <f t="shared" si="6"/>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="J42" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>556.61670598550438</v>
+        <v>556.62136163230343</v>
       </c>
       <c r="K42" s="19">
         <f t="shared" si="5"/>
@@ -6536,11 +6536,11 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="2"/>
-        <v>-76.630610472917994</v>
+        <v>23.272536028499761</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="3"/>
-        <v>457.94402252187012</v>
+        <v>557.84716902328785</v>
       </c>
       <c r="G43" s="18">
         <f t="shared" si="6"/>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="J43" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>545.47390146621308</v>
+        <v>545.48579064923013</v>
       </c>
       <c r="K43" s="19">
         <f t="shared" si="5"/>
@@ -6577,11 +6577,11 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="2"/>
-        <v>-21.231059287514068</v>
+        <v>80.149641700463462</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="3"/>
-        <v>502.65208104737826</v>
+        <v>604.03278203535581</v>
       </c>
       <c r="G44" s="18">
         <f t="shared" si="6"/>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="J44" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>534.57098440829441</v>
+        <v>534.58257171049229</v>
       </c>
       <c r="K44" s="19">
         <f t="shared" si="5"/>
@@ -6622,11 +6622,11 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="2"/>
-        <v>-23.195267264096742</v>
+        <v>-50.399356255169373</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="3"/>
-        <v>490.21021026409778</v>
+        <v>463.00612127302514</v>
       </c>
       <c r="G45" s="18">
         <f t="shared" si="6"/>
@@ -6642,7 +6642,7 @@
       </c>
       <c r="J45" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>523.87944407866485</v>
+        <v>523.87645790302963</v>
       </c>
       <c r="K45" s="19">
         <f t="shared" si="5"/>
@@ -6667,11 +6667,11 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="2"/>
-        <v>21.472274749746813</v>
+        <v>55.910986295682498</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="3"/>
-        <v>524.60964272737738</v>
+        <v>559.04835427331307</v>
       </c>
       <c r="G46" s="18">
         <f t="shared" si="6"/>
@@ -6687,7 +6687,7 @@
       </c>
       <c r="J46" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>513.40665870443809</v>
+        <v>513.41028933529867</v>
       </c>
       <c r="K46" s="19">
         <f t="shared" si="5"/>
@@ -6712,11 +6712,11 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3195072234434289</v>
+        <v>37.040190326433475</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="3"/>
-        <v>497.39412784152142</v>
+        <v>530.11481094451142</v>
       </c>
       <c r="G47" s="18">
         <f t="shared" si="6"/>
@@ -6732,7 +6732,7 @@
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>503.13678648242302</v>
+        <v>503.14009940682854</v>
       </c>
       <c r="K47" s="19">
         <f t="shared" si="5"/>
@@ -6757,11 +6757,11 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.6639142477469138</v>
+        <v>55.21580091269086</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="3"/>
-        <v>477.54921395796953</v>
+        <v>538.42892911840727</v>
       </c>
       <c r="G48" s="18">
         <f t="shared" si="6"/>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>493.07311093411488</v>
+        <v>493.07903085181289</v>
       </c>
       <c r="K48" s="19">
         <f t="shared" si="5"/>
@@ -6802,11 +6802,11 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="2"/>
-        <v>-2.2939476091915432</v>
+        <v>14.80089408486146</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="3"/>
-        <v>471.25491803241056</v>
+        <v>488.34975972646356</v>
       </c>
       <c r="G49" s="18">
         <f t="shared" si="6"/>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="J49" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>483.21201143745446</v>
+        <v>483.21360791187419</v>
       </c>
       <c r="K49" s="19">
         <f t="shared" si="5"/>
@@ -6847,11 +6847,11 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="2"/>
-        <v>11.991269278058846</v>
+        <v>-6.3862143952128498</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="3"/>
-        <v>476.06915760682887</v>
+        <v>457.69167393355718</v>
       </c>
       <c r="G50" s="18">
         <f t="shared" si="6"/>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>473.54909169003116</v>
+        <v>473.54744338841692</v>
       </c>
       <c r="K50" s="19">
         <f t="shared" si="5"/>
@@ -6892,11 +6892,11 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="2"/>
-        <v>20.672421509962742</v>
+        <v>88.332983205462725</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="3"/>
-        <v>475.46875207215737</v>
+        <v>543.12931376765732</v>
       </c>
       <c r="G51" s="18">
         <f t="shared" si="6"/>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="J51" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>464.07886953656379</v>
+        <v>464.08469781016635</v>
       </c>
       <c r="K51" s="19">
         <f t="shared" si="5"/>
@@ -6937,11 +6937,11 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="2"/>
-        <v>117.11600696917334</v>
+        <v>71.331636876944387</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="3"/>
-        <v>562.8164109201241</v>
+        <v>517.03204082789512</v>
       </c>
       <c r="G52" s="18">
         <f t="shared" si="6"/>
@@ -6957,7 +6957,7 @@
       </c>
       <c r="J52" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>454.80526695933906</v>
+        <v>454.80147926252567</v>
       </c>
       <c r="K52" s="19">
         <f t="shared" si="5"/>
@@ -6982,11 +6982,11 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.8433791740551986</v>
+        <v>-7.8498703310087308</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="3"/>
-        <v>434.94301669787649</v>
+        <v>428.93652554092296</v>
       </c>
       <c r="G53" s="18">
         <f t="shared" si="6"/>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="J53" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>445.69954924182241</v>
+        <v>445.69907200671878</v>
       </c>
       <c r="K53" s="19">
         <f t="shared" si="5"/>
@@ -7027,11 +7027,11 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="2"/>
-        <v>115.90170483248599</v>
+        <v>16.408255700510086</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="3"/>
-        <v>543.95237278697903</v>
+        <v>444.45892365500316</v>
       </c>
       <c r="G54" s="18">
         <f t="shared" si="6"/>
@@ -7047,7 +7047,7 @@
       </c>
       <c r="J54" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>436.79457339888774</v>
+        <v>436.78698134042247</v>
       </c>
       <c r="K54" s="19">
         <f t="shared" si="5"/>
@@ -7072,11 +7072,11 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="2"/>
-        <v>-18.441135210808078</v>
+        <v>2.2467037545803286</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="3"/>
-        <v>401.04851938459512</v>
+        <v>421.7363583499835</v>
       </c>
       <c r="G55" s="18">
         <f t="shared" si="6"/>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="J55" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>428.04868908641265</v>
+        <v>428.05020520666045</v>
       </c>
       <c r="K55" s="19">
         <f t="shared" si="5"/>
@@ -7117,11 +7117,11 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="2"/>
-        <v>-2.5507425801935804</v>
+        <v>76.804094711018962</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="3"/>
-        <v>408.54911892330153</v>
+        <v>487.9039562145141</v>
       </c>
       <c r="G56" s="18">
         <f t="shared" si="6"/>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="J56" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>419.48888456030801</v>
+        <v>419.49446984529942</v>
       </c>
       <c r="K56" s="19">
         <f t="shared" si="5"/>
@@ -7162,11 +7162,11 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="2"/>
-        <v>-30.780337712576994</v>
+        <v>-76.422157306822697</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="3"/>
-        <v>372.09752656084822</v>
+        <v>326.45570696660252</v>
       </c>
       <c r="G57" s="18">
         <f t="shared" si="6"/>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="J57" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>411.09722507557626</v>
+        <v>411.09413984061223</v>
       </c>
       <c r="K57" s="19">
         <f t="shared" si="5"/>
@@ -7207,11 +7207,11 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="2"/>
-        <v>27.099136463620326</v>
+        <v>82.935916148527127</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="3"/>
-        <v>421.91944345157697</v>
+        <v>477.75622313648375</v>
       </c>
       <c r="G58" s="18">
         <f t="shared" si="6"/>
@@ -7227,7 +7227,7 @@
       </c>
       <c r="J58" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>402.87910045302203</v>
+        <v>402.8827253775703</v>
       </c>
       <c r="K58" s="19">
         <f t="shared" si="5"/>
@@ -7248,11 +7248,11 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="2"/>
-        <v>14.012257216846166</v>
+        <v>-50.020986121940624</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="3"/>
-        <v>400.93615806504363</v>
+        <v>336.90291472625688</v>
       </c>
       <c r="G59" s="18">
         <f t="shared" si="6"/>
@@ -7268,7 +7268,7 @@
       </c>
       <c r="J59" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>394.82068830724853</v>
+        <v>394.81669587664481</v>
       </c>
       <c r="K59" s="19">
         <f t="shared" si="5"/>
@@ -7289,11 +7289,11 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="2"/>
-        <v>56.874272920815962</v>
+        <v>18.34637012579411</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="3"/>
-        <v>436.05969575204949</v>
+        <v>397.53179295702768</v>
       </c>
       <c r="G60" s="18">
         <f t="shared" si="6"/>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="J60" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>386.9268431220089</v>
+        <v>386.92453605361561</v>
       </c>
       <c r="K60" s="19">
         <f t="shared" si="5"/>
@@ -7330,11 +7330,11 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="2"/>
-        <v>-69.999546429976689</v>
+        <v>-51.413208921494849</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="3"/>
-        <v>301.60216794463219</v>
+        <v>320.18850545311403</v>
       </c>
       <c r="G61" s="18">
         <f t="shared" si="6"/>
@@ -7350,7 +7350,7 @@
       </c>
       <c r="J61" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>379.18096107050184</v>
+        <v>379.18202995825294</v>
       </c>
       <c r="K61" s="19">
         <f t="shared" si="5"/>
@@ -7371,11 +7371,11 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.1333998553589364</v>
+        <v>-12.820145450106221</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="3"/>
-        <v>359.03628023175776</v>
+        <v>351.34953463701049</v>
       </c>
       <c r="G62" s="18">
         <f t="shared" si="6"/>
@@ -7391,7 +7391,7 @@
       </c>
       <c r="J62" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>371.60102035950865</v>
+        <v>371.60059580453873</v>
       </c>
       <c r="K62" s="19">
         <f t="shared" si="5"/>
@@ -7412,11 +7412,11 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="2"/>
-        <v>39.947777853869262</v>
+        <v>-8.7186365185462709</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="3"/>
-        <v>396.83406433924364</v>
+        <v>348.16764996682815</v>
       </c>
       <c r="G63" s="18">
         <f t="shared" si="6"/>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="J63" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>364.17141276965492</v>
+        <v>364.168831259294</v>
       </c>
       <c r="K63" s="19">
         <f t="shared" si="5"/>
@@ -7453,11 +7453,11 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="2"/>
-        <v>68.618753978255981</v>
+        <v>58.259856185174627</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="3"/>
-        <v>418.36731473392291</v>
+        <v>408.00841694084153</v>
       </c>
       <c r="G64" s="18">
         <f t="shared" si="6"/>
@@ -7473,7 +7473,7 @@
       </c>
       <c r="J64" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>356.88941860765397</v>
+        <v>356.88889087844228</v>
       </c>
       <c r="K64" s="19">
         <f t="shared" si="5"/>
@@ -7494,11 +7494,11 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="2"/>
-        <v>-81.126729638574417</v>
+        <v>-1.5096760739819133</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="3"/>
-        <v>261.62685990197912</v>
+        <v>341.24391346657166</v>
       </c>
       <c r="G65" s="18">
         <f t="shared" si="6"/>
@@ -7514,7 +7514,7 @@
       </c>
       <c r="J65" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>349.74424920509023</v>
+        <v>349.74814464684732</v>
       </c>
       <c r="K65" s="19">
         <f t="shared" si="5"/>
@@ -7535,11 +7535,11 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="2"/>
-        <v>48.03298035252223</v>
+        <v>-36.070481543752685</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="3"/>
-        <v>383.93149810226475</v>
+        <v>299.8280362059898</v>
       </c>
       <c r="G66" s="18">
         <f t="shared" si="6"/>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="J66" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>342.75552448228706</v>
+        <v>342.75157247733972</v>
       </c>
       <c r="K66" s="19">
         <f t="shared" si="5"/>
@@ -7576,11 +7576,11 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="2"/>
-        <v>40.066565973129251</v>
+        <v>-32.570016665553943</v>
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="3"/>
-        <v>369.24711336787686</v>
+        <v>296.61053072919367</v>
       </c>
       <c r="G67" s="18">
         <f t="shared" si="6"/>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="J67" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>335.900022741481</v>
+        <v>335.89674471868102</v>
       </c>
       <c r="K67" s="19">
         <f t="shared" si="5"/>
@@ -7617,11 +7617,11 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>71.553726894496009</v>
+        <v>24.691826821663419</v>
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="3"/>
-        <v>394.15066334134872</v>
+        <v>347.28876326851611</v>
       </c>
       <c r="G68" s="18">
         <f t="shared" si="6"/>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="J68" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>329.18336333305376</v>
+        <v>329.18133224202688</v>
       </c>
       <c r="K68" s="19">
         <f t="shared" si="5"/>
@@ -7658,11 +7658,11 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.5402893820015862</v>
+        <v>-58.653052927555592</v>
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="3"/>
-        <v>314.60470833591404</v>
+        <v>257.49194479035998</v>
       </c>
       <c r="G69" s="18">
         <f t="shared" si="6"/>
@@ -7678,7 +7678,7 @@
       </c>
       <c r="J69" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>322.59660376411898</v>
+        <v>322.59422640075508</v>
       </c>
       <c r="K69" s="19">
         <f t="shared" si="5"/>
@@ -7699,11 +7699,11 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="2"/>
-        <v>1.720909295692771</v>
+        <v>-3.5776186081183754</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="3"/>
-        <v>311.54300705925004</v>
+        <v>306.24447915543891</v>
       </c>
       <c r="G70" s="18">
         <f t="shared" si="6"/>
@@ -7719,7 +7719,7 @@
       </c>
       <c r="J70" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>316.14481374199249</v>
+        <v>316.14460192027565</v>
       </c>
       <c r="K70" s="19">
         <f t="shared" si="5"/>
@@ -7740,11 +7740,11 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="2"/>
-        <v>-17.594753501794276</v>
+        <v>51.346276769176832</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="3"/>
-        <v>286.03090230649184</v>
+        <v>354.97193257746295</v>
       </c>
       <c r="G71" s="18">
         <f t="shared" si="6"/>
@@ -7760,7 +7760,7 @@
       </c>
       <c r="J71" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>309.82118431443712</v>
+        <v>309.82383126522012</v>
       </c>
       <c r="K71" s="19">
         <f t="shared" si="5"/>
@@ -7781,11 +7781,11 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="2"/>
-        <v>66.219555980677569</v>
+        <v>52.189732922261697</v>
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="3"/>
-        <v>363.77269867279796</v>
+        <v>349.74287561438211</v>
       </c>
       <c r="G72" s="18">
         <f t="shared" si="6"/>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="J72" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>303.62787367370089</v>
+        <v>303.62735633722258</v>
       </c>
       <c r="K72" s="19">
         <f t="shared" si="5"/>
@@ -7822,11 +7822,11 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="2"/>
-        <v>-48.068431880745543</v>
+        <v>-35.252545663830922</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="3"/>
-        <v>243.53364795753242</v>
+        <v>256.34953417444706</v>
       </c>
       <c r="G73" s="18">
         <f t="shared" si="6"/>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="J73" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>297.55122965141118</v>
+        <v>297.55168351185876</v>
       </c>
       <c r="K73" s="19">
         <f t="shared" si="5"/>
@@ -7863,11 +7863,11 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="2"/>
-        <v>-33.648551971642306</v>
+        <v>22.882581289836207</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="3"/>
-        <v>252.1214862698701</v>
+        <v>308.65261953134859</v>
       </c>
       <c r="G74" s="18">
         <f t="shared" si="6"/>
@@ -7883,7 +7883,7 @@
       </c>
       <c r="J74" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>291.60073704200255</v>
+        <v>291.60265975360153</v>
       </c>
       <c r="K74" s="19">
         <f t="shared" si="5"/>
@@ -7904,11 +7904,11 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="2"/>
-        <v>-33.576196391944968</v>
+        <v>-11.959365541245218</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="3"/>
-        <v>246.4784410847372</v>
+        <v>268.09527193543693</v>
       </c>
       <c r="G75" s="18">
         <f t="shared" si="6"/>
@@ -7924,7 +7924,7 @@
       </c>
       <c r="J75" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>285.76875479175101</v>
+        <v>285.76946089988621</v>
       </c>
       <c r="K75" s="19">
         <f t="shared" si="5"/>
@@ -7945,11 +7945,11 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="2"/>
-        <v>-21.57197853077902</v>
+        <v>-22.019132247466558</v>
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="3"/>
-        <v>252.88156619636953</v>
+        <v>252.43441247968198</v>
       </c>
       <c r="G76" s="18">
         <f t="shared" si="6"/>
@@ -7965,7 +7965,7 @@
       </c>
       <c r="J76" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>280.05378502331212</v>
+        <v>280.05377099553846</v>
       </c>
       <c r="K76" s="19">
         <f t="shared" si="5"/>
@@ -7986,11 +7986,11 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="2"/>
-        <v>41.228059965845141</v>
+        <v>-23.566556643576032</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="3"/>
-        <v>310.19253379845071</v>
+        <v>245.39791718902953</v>
       </c>
       <c r="G77" s="18">
         <f t="shared" si="6"/>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="J77" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>274.45462150684654</v>
+        <v>274.45266931039339</v>
       </c>
       <c r="K77" s="19">
         <f t="shared" si="5"/>
@@ -8027,11 +8027,11 @@
       </c>
       <c r="E78">
         <f t="shared" ref="E78:E113" ca="1" si="10">IF($K$3=0,$K$2,NORMINV(RAND(),$K$2,$K$3))</f>
-        <v>76.046074279572878</v>
+        <v>-12.840352648919445</v>
       </c>
       <c r="F78">
         <f t="shared" ref="F78:F113" ca="1" si="11">D78+E78</f>
-        <v>339.63125863552636</v>
+        <v>250.74483170703402</v>
       </c>
       <c r="G78" s="18">
         <f t="shared" si="6"/>
@@ -8047,7 +8047,7 @@
       </c>
       <c r="J78" s="9">
         <f t="shared" ref="J78:J113" ca="1" si="12">G78+I78*(F78-G78)</f>
-        <v>268.96651864089324</v>
+        <v>268.9639466305357</v>
       </c>
       <c r="K78" s="19">
         <f t="shared" ref="K78:K113" si="13">(1-I78)*H78</f>
@@ -8068,11 +8068,11 @@
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="10"/>
-        <v>-42.022713078187955</v>
+        <v>-33.686249047580816</v>
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="11"/>
-        <v>216.2907675906464</v>
+        <v>224.62723162125354</v>
       </c>
       <c r="G79" s="18">
         <f t="shared" ref="G79:G113" si="14">$B$2*G78</f>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="J79" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>263.58387003997547</v>
+        <v>263.58410171103992</v>
       </c>
       <c r="K79" s="19">
         <f t="shared" si="13"/>
@@ -8109,11 +8109,11 @@
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="10"/>
-        <v>-8.035417742567299</v>
+        <v>33.511600818433685</v>
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="11"/>
-        <v>245.11179331289037</v>
+        <v>286.65881187389135</v>
       </c>
       <c r="G80" s="18">
         <f t="shared" si="14"/>
@@ -8129,7 +8129,7 @@
       </c>
       <c r="J80" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>258.31312832069187</v>
+        <v>258.31423719521837</v>
       </c>
       <c r="K80" s="19">
         <f t="shared" si="13"/>
@@ -8150,11 +8150,11 @@
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="10"/>
-        <v>20.014589130869297</v>
+        <v>128.63591991082038</v>
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="11"/>
-        <v>268.09885596521781</v>
+        <v>376.72018674516892</v>
       </c>
       <c r="G81" s="18">
         <f t="shared" si="14"/>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="J81" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>253.14759430719084</v>
+        <v>253.1503785702958</v>
       </c>
       <c r="K81" s="19">
         <f t="shared" si="13"/>
@@ -8191,11 +8191,11 @@
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="10"/>
-        <v>-129.1326761048056</v>
+        <v>9.9167076110071157</v>
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="11"/>
-        <v>113.98990539285595</v>
+        <v>253.03928910866867</v>
       </c>
       <c r="G82" s="18">
         <f t="shared" si="14"/>
@@ -8211,7 +8211,7 @@
       </c>
       <c r="J82" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>248.08096573753073</v>
+        <v>248.08438881567633</v>
       </c>
       <c r="K82" s="19">
         <f t="shared" si="13"/>
@@ -8232,11 +8232,11 @@
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="10"/>
-        <v>-19.388886371823162</v>
+        <v>5.7403102879881489</v>
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="11"/>
-        <v>218.87124349588515</v>
+        <v>244.00044015569645</v>
       </c>
       <c r="G83" s="18">
         <f t="shared" si="14"/>
@@ -8252,7 +8252,7 @@
       </c>
       <c r="J83" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>243.12200812626361</v>
+        <v>243.12260225276569</v>
       </c>
       <c r="K83" s="19">
         <f t="shared" si="13"/>
@@ -8273,11 +8273,11 @@
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.73666853808857025</v>
+        <v>30.56930618246647</v>
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="11"/>
-        <v>232.75825873226557</v>
+        <v>264.06423345282059</v>
       </c>
       <c r="G84" s="18">
         <f t="shared" si="14"/>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="J84" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>238.26000493870006</v>
+        <v>238.26071579220385</v>
       </c>
       <c r="K84" s="19">
         <f t="shared" si="13"/>
@@ -8314,11 +8314,11 @@
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="10"/>
-        <v>0.16291370999054811</v>
+        <v>-9.649541762151042</v>
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="11"/>
-        <v>228.98794243493762</v>
+        <v>219.17548696279601</v>
       </c>
       <c r="G85" s="18">
         <f t="shared" si="14"/>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="J85" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>233.49482898438669</v>
+        <v>233.49461499949115</v>
       </c>
       <c r="K85" s="19">
         <f t="shared" si="13"/>
@@ -8355,11 +8355,11 @@
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="10"/>
-        <v>-23.479539893006265</v>
+        <v>-89.047864642919222</v>
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="11"/>
-        <v>200.76898825744186</v>
+        <v>135.2006635075289</v>
       </c>
       <c r="G86" s="18">
         <f t="shared" si="14"/>
@@ -8375,7 +8375,7 @@
       </c>
       <c r="J86" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>228.82444112151222</v>
+        <v>228.82306786383944</v>
       </c>
       <c r="K86" s="19">
         <f t="shared" si="13"/>
@@ -8396,11 +8396,11 @@
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="10"/>
-        <v>-27.154608482818134</v>
+        <v>-27.749751222169738</v>
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="11"/>
-        <v>192.60894910462102</v>
+        <v>192.0138063652694</v>
       </c>
       <c r="G87" s="18">
         <f t="shared" si="14"/>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="J87" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>224.24789173435261</v>
+        <v>224.24787976332044</v>
       </c>
       <c r="K87" s="19">
         <f t="shared" si="13"/>
@@ -8437,11 +8437,11 @@
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="10"/>
-        <v>8.922060064594012</v>
+        <v>47.982788583732564</v>
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="11"/>
-        <v>224.29034650028439</v>
+        <v>263.35107501942292</v>
       </c>
       <c r="G88" s="18">
         <f t="shared" si="14"/>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="J88" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>219.76364503610719</v>
+        <v>219.76439961263969</v>
       </c>
       <c r="K88" s="19">
         <f t="shared" si="13"/>
@@ -8478,11 +8478,11 @@
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="10"/>
-        <v>25.118505151045884</v>
+        <v>4.1022595735456191</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="11"/>
-        <v>236.17942585802246</v>
+        <v>215.16318028052217</v>
       </c>
       <c r="G89" s="18">
         <f t="shared" si="14"/>
@@ -8498,7 +8498,7 @@
       </c>
       <c r="J89" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>215.3686725459109</v>
+        <v>215.36828263034454</v>
       </c>
       <c r="K89" s="19">
         <f t="shared" si="13"/>
@@ -8519,11 +8519,11 @@
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="10"/>
-        <v>30.954677383587857</v>
+        <v>42.812736378424738</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="11"/>
-        <v>237.79437967642488</v>
+        <v>249.65243867126176</v>
       </c>
       <c r="G90" s="18">
         <f t="shared" si="14"/>
@@ -8539,7 +8539,7 @@
       </c>
       <c r="J90" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>211.06139705357035</v>
+        <v>211.06160834482216</v>
       </c>
       <c r="K90" s="19">
         <f t="shared" si="13"/>
@@ -8560,11 +8560,11 @@
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="10"/>
-        <v>-27.403969419911249</v>
+        <v>15.979445769171846</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="11"/>
-        <v>175.29893882706904</v>
+        <v>218.68235401615215</v>
       </c>
       <c r="G91" s="18">
         <f t="shared" si="14"/>
@@ -8580,7 +8580,7 @@
       </c>
       <c r="J91" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>206.83916254293916</v>
+        <v>206.83990495343733</v>
       </c>
       <c r="K91" s="19">
         <f t="shared" si="13"/>
@@ -8601,11 +8601,11 @@
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="10"/>
-        <v>119.75955763818156</v>
+        <v>-56.682095580539652</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="11"/>
-        <v>318.40840772022221</v>
+        <v>141.96675450150101</v>
       </c>
       <c r="G92" s="18">
         <f t="shared" si="14"/>
@@ -8621,7 +8621,7 @@
       </c>
       <c r="J92" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>202.70480988045804</v>
+        <v>202.70191004115776</v>
       </c>
       <c r="K92" s="19">
         <f t="shared" si="13"/>
@@ -8642,11 +8642,11 @@
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="10"/>
-        <v>-75.554829149295543</v>
+        <v>-38.037477024533558</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="11"/>
-        <v>119.1210439311043</v>
+        <v>156.63839605586628</v>
       </c>
       <c r="G93" s="18">
         <f t="shared" si="14"/>
@@ -8662,7 +8662,7 @@
       </c>
       <c r="J93" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>198.64759479152008</v>
+        <v>198.64818697655269</v>
       </c>
       <c r="K93" s="19">
         <f t="shared" si="13"/>
@@ -8683,11 +8683,11 @@
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="10"/>
-        <v>7.687242018671518</v>
+        <v>83.909503618019571</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="11"/>
-        <v>198.46959763746335</v>
+        <v>274.69185923681141</v>
       </c>
       <c r="G94" s="18">
         <f t="shared" si="14"/>
@@ -8703,7 +8703,7 @@
       </c>
       <c r="J94" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>194.67593059041283</v>
+        <v>194.67708606261135</v>
       </c>
       <c r="K94" s="19">
         <f t="shared" si="13"/>
@@ -8724,11 +8724,11 @@
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="10"/>
-        <v>55.374561999592409</v>
+        <v>-135.47105257336918</v>
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="11"/>
-        <v>242.34127050600839</v>
+        <v>51.495655933046805</v>
       </c>
       <c r="G95" s="18">
         <f t="shared" si="14"/>
@@ -8744,7 +8744,7 @@
       </c>
       <c r="J95" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>190.78310626250317</v>
+        <v>190.7803277505673</v>
       </c>
       <c r="K95" s="19">
         <f t="shared" si="13"/>
@@ -8765,11 +8765,11 @@
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="10"/>
-        <v>-103.22080189807772</v>
+        <v>74.181366184336824</v>
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="11"/>
-        <v>80.006572438209929</v>
+        <v>257.40874052062446</v>
       </c>
       <c r="G96" s="18">
         <f t="shared" si="14"/>
@@ -8785,7 +8785,7 @@
       </c>
       <c r="J96" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>186.96521294438622</v>
+        <v>186.96769345681201</v>
       </c>
       <c r="K96" s="19">
         <f t="shared" si="13"/>
@@ -8806,11 +8806,11 @@
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="10"/>
-        <v>-32.460027154485559</v>
+        <v>18.544076595943437</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="11"/>
-        <v>147.10279969507633</v>
+        <v>198.10690344550534</v>
       </c>
       <c r="G97" s="18">
         <f t="shared" si="14"/>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="J97" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>183.2268892292025</v>
+        <v>183.22757414943607</v>
       </c>
       <c r="K97" s="19">
         <f t="shared" si="13"/>
@@ -8847,11 +8847,11 @@
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="10"/>
-        <v>-42.236349198780175</v>
+        <v>-16.790000494652801</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="11"/>
-        <v>133.73522111379049</v>
+        <v>159.18156981791788</v>
       </c>
       <c r="G98" s="18">
         <f t="shared" si="14"/>
@@ -8867,7 +8867,7 @@
       </c>
       <c r="J98" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>179.56223581289302</v>
+        <v>179.56256399336266</v>
       </c>
       <c r="K98" s="19">
         <f t="shared" si="13"/>
@@ -8888,11 +8888,11 @@
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="10"/>
-        <v>44.489402142689258</v>
+        <v>2.3834328575389341</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="11"/>
-        <v>216.94154104900849</v>
+        <v>174.83557176385818</v>
       </c>
       <c r="G99" s="18">
         <f t="shared" si="14"/>
@@ -8908,7 +8908,7 @@
       </c>
       <c r="J99" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>175.97207777662499</v>
+        <v>175.97155624181545</v>
       </c>
       <c r="K99" s="19">
         <f t="shared" si="13"/>
@@ -8929,11 +8929,11 @@
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="10"/>
-        <v>10.90664451367215</v>
+        <v>-91.818088258537841</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="11"/>
-        <v>179.909740641865</v>
+        <v>77.18500786965501</v>
       </c>
       <c r="G100" s="18">
         <f t="shared" si="14"/>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="J100" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>172.4522276201192</v>
+        <v>172.4510056319094</v>
       </c>
       <c r="K100" s="19">
         <f t="shared" si="13"/>
@@ -8970,11 +8970,11 @@
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="10"/>
-        <v>8.4199517084491955</v>
+        <v>-17.550711049221732</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="11"/>
-        <v>174.04298591407817</v>
+        <v>148.07232315640726</v>
       </c>
       <c r="G101" s="18">
         <f t="shared" si="14"/>
@@ -8990,7 +8990,7 @@
       </c>
       <c r="J101" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>169.00315370736158</v>
+        <v>169.00285700064046</v>
       </c>
       <c r="K101" s="19">
         <f t="shared" si="13"/>
@@ -9011,11 +9011,11 @@
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="10"/>
-        <v>48.552586743722514</v>
+        <v>-62.835330326649128</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="11"/>
-        <v>210.86316026523892</v>
+        <v>99.475243194867275</v>
       </c>
       <c r="G102" s="18">
         <f t="shared" si="14"/>
@@ -9031,7 +9031,7 @@
       </c>
       <c r="J102" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>165.62353059275085</v>
+        <v>165.62230841384945</v>
       </c>
       <c r="K102" s="19">
         <f t="shared" si="13"/>
@@ -9052,11 +9052,11 @@
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="10"/>
-        <v>74.663949141063796</v>
+        <v>60.976630077951121</v>
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="11"/>
-        <v>233.72831119214987</v>
+        <v>220.04099212903719</v>
       </c>
       <c r="G103" s="18">
         <f t="shared" si="14"/>
@@ -9072,7 +9072,7 @@
       </c>
       <c r="J103" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>162.31132610577157</v>
+        <v>162.31118187184373</v>
       </c>
       <c r="K103" s="19">
         <f t="shared" si="13"/>
@@ -9093,11 +9093,11 @@
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="10"/>
-        <v>-61.233909364490358</v>
+        <v>-123.43128058352963</v>
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="11"/>
-        <v>94.649165445573999</v>
+        <v>32.45179422653473</v>
       </c>
       <c r="G104" s="18">
         <f t="shared" si="14"/>
@@ -9113,7 +9113,7 @@
       </c>
       <c r="J104" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>159.0637101379852</v>
+        <v>159.06308067035528</v>
       </c>
       <c r="K104" s="19">
         <f t="shared" si="13"/>
@@ -9134,11 +9134,11 @@
       </c>
       <c r="E105">
         <f t="shared" ca="1" si="10"/>
-        <v>-23.226915585558523</v>
+        <v>20.423526321728495</v>
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="11"/>
-        <v>129.53849772830455</v>
+        <v>173.18893963559157</v>
       </c>
       <c r="G105" s="18">
         <f t="shared" si="14"/>
@@ -9154,7 +9154,7 @@
       </c>
       <c r="J105" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>155.88281874818503</v>
+        <v>155.88324301820285</v>
       </c>
       <c r="K105" s="19">
         <f t="shared" si="13"/>
@@ -9175,11 +9175,11 @@
       </c>
       <c r="E106">
         <f t="shared" ca="1" si="10"/>
-        <v>3.982838378547942</v>
+        <v>-21.012034400637646</v>
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="11"/>
-        <v>153.69294342613375</v>
+        <v>128.69807064694817</v>
       </c>
       <c r="G106" s="18">
         <f t="shared" si="14"/>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="J106" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>152.76542197219106</v>
+        <v>152.7651886495162</v>
       </c>
       <c r="K106" s="19">
         <f t="shared" si="13"/>
@@ -9216,11 +9216,11 @@
       </c>
       <c r="E107">
         <f t="shared" ca="1" si="10"/>
-        <v>-72.069730991542116</v>
+        <v>-43.170893110404883</v>
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="11"/>
-        <v>74.646171955091972</v>
+        <v>103.54500983622921</v>
       </c>
       <c r="G107" s="18">
         <f t="shared" si="14"/>
@@ -9236,7 +9236,7 @@
       </c>
       <c r="J107" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>149.70943208697656</v>
+        <v>149.70969116985091</v>
       </c>
       <c r="K107" s="19">
         <f t="shared" si="13"/>
@@ -9257,11 +9257,11 @@
       </c>
       <c r="E108">
         <f t="shared" ca="1" si="10"/>
-        <v>-4.6481869734118986</v>
+        <v>-37.994269357075076</v>
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="11"/>
-        <v>139.1333979142895</v>
+        <v>105.78731553062633</v>
       </c>
       <c r="G108" s="18">
         <f t="shared" si="14"/>
@@ -9277,7 +9277,7 @@
       </c>
       <c r="J108" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>146.71583766014101</v>
+        <v>146.71555054542526</v>
       </c>
       <c r="K108" s="19">
         <f t="shared" si="13"/>
@@ -9298,11 +9298,11 @@
       </c>
       <c r="E109">
         <f t="shared" ca="1" si="10"/>
-        <v>-26.662846004574124</v>
+        <v>60.917106492565878</v>
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="11"/>
-        <v>114.24310718537326</v>
+        <v>201.82305968251325</v>
       </c>
       <c r="G109" s="18">
         <f t="shared" si="14"/>
@@ -9318,7 +9318,7 @@
       </c>
       <c r="J109" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>143.78134062843822</v>
+        <v>143.78206484364264</v>
       </c>
       <c r="K109" s="19">
         <f t="shared" si="13"/>
@@ -9339,11 +9339,11 @@
       </c>
       <c r="E110">
         <f t="shared" ca="1" si="10"/>
-        <v>-121.38979849519951</v>
+        <v>-2.2789522726189575</v>
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="11"/>
-        <v>16.698035630948922</v>
+        <v>135.80888185352947</v>
       </c>
       <c r="G110" s="18">
         <f t="shared" si="14"/>
@@ -9359,7 +9359,7 @@
       </c>
       <c r="J110" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>140.90496676395557</v>
+        <v>140.90591271037292</v>
       </c>
       <c r="K110" s="19">
         <f t="shared" si="13"/>
@@ -9380,11 +9380,11 @@
       </c>
       <c r="E111">
         <f t="shared" ca="1" si="10"/>
-        <v>-40.912435884728488</v>
+        <v>15.826818590013444</v>
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="11"/>
-        <v>94.413641558896984</v>
+        <v>151.15289603363891</v>
       </c>
       <c r="G111" s="18">
         <f t="shared" si="14"/>
@@ -9400,7 +9400,7 @@
       </c>
       <c r="J111" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>138.08750101252139</v>
+        <v>138.08793377653473</v>
       </c>
       <c r="K111" s="19">
         <f t="shared" si="13"/>
@@ -9421,11 +9421,11 @@
       </c>
       <c r="E112">
         <f t="shared" ca="1" si="10"/>
-        <v>-103.32370286993817</v>
+        <v>9.2409163713480069</v>
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="11"/>
-        <v>29.295853024814804</v>
+        <v>141.860472266101</v>
       </c>
       <c r="G112" s="18">
         <f t="shared" si="14"/>
@@ -9441,7 +9441,7 @@
       </c>
       <c r="J112" s="9">
         <f t="shared" ca="1" si="12"/>
-        <v>135.32530075047043</v>
+        <v>135.32612530940864</v>
       </c>
       <c r="K112" s="19">
         <f t="shared" si="13"/>
@@ -9462,11 +9462,11 @@
       </c>
       <c r="E113">
         <f t="shared" ca="1" si="10"/>
-        <v>-7.185026524589694</v>
+        <v>-15.869639478674975</v>
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="11"/>
-        <v>122.78213825226823</v>
+        <v>114.09752529818294</v>
       </c>
       <c r="G113" s="28">
         <f t="shared" si="14"/>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="J113" s="29">
         <f t="shared" ca="1" si="12"/>
-        <v>132.61948668724938</v>
+        <v>132.61942558987562</v>
       </c>
       <c r="K113" s="30">
         <f t="shared" si="13"/>

</xml_diff>